<commit_message>
authorisatie gefixt, CSS en JS gefixt, logout knop toegevoegd, begin van pagina voor toevoegen klusje gamaakt. Klasse postit gemaakt. Alle klassen voor registratie gebruiker via RestAPI gemaakt, maar nog een error
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d5897c9615995d8/hogeschool/semester 7/ApplicatieArchete/ProjectAppArch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelte\Documents\KUL\AppArch\Project\ProjectAppArch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{59D2DB9E-48B4-47A6-BAAE-07694E0D2306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78663AFC-B227-45F4-940A-BC10031818A7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E383AFF5-B836-4BE1-AA17-EEE7CF78B918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11295" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Naam student 2:</t>
   </si>
@@ -58,12 +58,24 @@
   </si>
   <si>
     <t>opzetten database, eerste securty toevoeging, login dat leest uit database en start van registeren (nog niet af)</t>
+  </si>
+  <si>
+    <t>Github repo aangemaakt met Spring project</t>
+  </si>
+  <si>
+    <t>Eerste GUI en proof of concept: Aanmaken index-, login- en registreerpagina. HTML + CSS en JS</t>
+  </si>
+  <si>
+    <t>Login authorisatie gefixt + doorverwijzingen controller. CSS gefixt + fragments. Logout knop toegevoegd. Alle klassen (repo,service,..) om gebruiker te registreren toegevoegd, maar nog probleem met toevoegen aan DB via restAPI. Tabel Customer aangepast om functie user mee op te slaan. Klasse voor klusjes aangemaakt, en begin van pagina om nieuwe klusjes toe te voegen.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -142,9 +154,11 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Kop 1" xfId="1" builtinId="16"/>
@@ -462,19 +476,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36EF922A-C188-1F43-B267-5D771EC01B6B}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="23.875" customWidth="1"/>
-    <col min="3" max="3" width="27.125" customWidth="1"/>
+    <col min="1" max="1" width="36.19921875" customWidth="1"/>
+    <col min="2" max="2" width="23.8984375" customWidth="1"/>
+    <col min="3" max="3" width="27.09765625" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
@@ -482,15 +496,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="9" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -504,317 +518,335 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:4" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6">
+        <v>45627</v>
+      </c>
+      <c r="C4" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6">
+        <v>45630</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B6" s="6">
         <v>45630</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8">
         <v>4.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+    <row r="7" spans="1:4" ht="163.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6">
+        <v>45633</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
       <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="5"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="5"/>
       <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="5"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="1"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="1"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="1"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="1"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="1"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="1"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="1"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="1"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D57" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Index pagina: Task prijs toegevoegd, postit kleur afhankelijk van status task in database. Add job knop veranderd naar een knop (met styling) ipv afbeelding. AddJob pagina: Styling gefixt + extra uitleg. Reroute naar index gefixt. Footer: Layout+kleur fix. Header: Menubalk styling gegeven en 'deftige' navigatie knoppen aangemaakt. Profiel Pagina: Styling toegevoegd. User kan naam zien en wijzigen in de DB. User kan ook zijn/haar klusjes bekijken, openstaande klusjes bovenaan, afgewerkte onderaan. Info Pagina: Aangemaakt volgens algemene styling, nog geen nuttige info in geplaatst.
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d5897c9615995d8/hogeschool/semester 7/ApplicatieArchete/ProjectAppArch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelte\Documents\KUL\AppArch\Project\ProjectAppArch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{E383AFF5-B836-4BE1-AA17-EEE7CF78B918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B5E29C4-3E3E-4835-8056-272C101F6F7E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B581327-3A61-4633-B01B-BB3EB1C66CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11295" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
+    <workbookView xWindow="3936" yWindow="372" windowWidth="19104" windowHeight="8880" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Naam student 2:</t>
   </si>
@@ -76,6 +76,134 @@
   </si>
   <si>
     <t xml:space="preserve">task aanmaken afmaken, task automaties index pagina laten tonen </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Index pagina</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Task prijs toegevoegd, postit kleur afhankelijk van status task in database. Add job knop veranderd naar een knop (met styling) ipv afbeelding. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AddJob pagina</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Styling gefixt + extra uitleg. Reroute naar index gefixt. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Footer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Layout+kleur fix. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Header</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Menubalk styling gegeven en 'deftige' navigatie knoppen aangemaakt. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Profiel Pagina</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Styling toegevoegd. User kan naam zien en wijzigen in de DB. User kan ook zijn/haar klusjes bekijken, openstaande klusjes bovenaan, afgewerkte onderaan. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Info Pagina</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Aangemaakt volgens algemene styling, nog geen nuttige info in geplaatst.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -85,7 +213,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -97,6 +225,14 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -485,19 +621,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36EF922A-C188-1F43-B267-5D771EC01B6B}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.25" customWidth="1"/>
-    <col min="2" max="2" width="23.875" customWidth="1"/>
-    <col min="3" max="3" width="27.125" customWidth="1"/>
+    <col min="1" max="1" width="36.19921875" customWidth="1"/>
+    <col min="2" max="2" width="23.8984375" customWidth="1"/>
+    <col min="3" max="3" width="27.09765625" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
@@ -505,7 +641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
@@ -513,7 +649,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -527,7 +663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
@@ -539,7 +675,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -551,7 +687,7 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -563,7 +699,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="163.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="163.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -575,7 +711,7 @@
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
@@ -587,7 +723,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -599,7 +735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -611,272 +747,279 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="8"/>
+    <row r="11" spans="1:4" ht="249.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="6">
+        <v>45637</v>
+      </c>
+      <c r="C11" s="8">
+        <v>5</v>
+      </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="6"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="1"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="1"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="1"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="1"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="1"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="1"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="1"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="1"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D57" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Profile Pagina: Klant en klusjesman krijgen verschillende pagina te zien waarop andere gegevens te vinden zijn [maincontroller]. Ook nieuwe beta querries toegevoegd om deze verschillende data op te halen [taskrepo]. LET OP: task heeft nog geen variabele voor geboden klanten en toegewezen klant. De queries zijn dus puur als test kwestie van voorbeeld.
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelte\Documents\KUL\AppArch\Project\ProjectAppArch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B581327-3A61-4633-B01B-BB3EB1C66CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A0BCD9-CD6A-4DEE-B4C2-C7B58EDF3D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3936" yWindow="372" windowWidth="19104" windowHeight="8880" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Naam student 2:</t>
   </si>
@@ -203,6 +203,71 @@
         <scheme val="minor"/>
       </rPr>
       <t>: Aangemaakt volgens algemene styling, nog geen nuttige info in geplaatst.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Profile Pagina</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Klant en klusjesman krijgen verschillende pagina te zien waarop andere gegevens te vinden zijn</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [maincontroller]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Ook nieuwe beta querries toegevoegd om deze verschillende data op te halen </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[taskrepo]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
     </r>
   </si>
 </sst>
@@ -213,7 +278,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,6 +296,14 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -622,7 +695,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -759,10 +832,16 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="8"/>
+    <row r="12" spans="1:4" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="6">
+        <v>45638</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.5</v>
+      </c>
       <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
klant kan persoon aan duiden die geboden heeft, index zodat op toegewezen taken niet meer kan geboden worden
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d5897c9615995d8/hogeschool/semester 7/ApplicatieArchete/ProjectAppArch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{75A0BCD9-CD6A-4DEE-B4C2-C7B58EDF3D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DAEF433-381D-45AC-95BC-E80652D933DF}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{75A0BCD9-CD6A-4DEE-B4C2-C7B58EDF3D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{360CC0A2-9AB0-41AD-821C-41C9230FF9B8}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15345" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Naam student 2:</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>Roles in aparte Table gestoken,passwoord encryptie toegevoegt, index pagina voor klusjesman en klant anders gemaakt zodat een klusjesman geen task kan maken, nieuwepagina gemaakt voor task aantepassen, , offer table gemaakt, je kan offer doen, het opslpitsen van code en het starten schrijven aan het selecteren van een user (verloopig 403 error)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">klant kan user aan duiden op taak, taak waar een toewijzing op gebeurd kan niet meer geboden op worden en komen achteraan op de bord te staan. </t>
   </si>
 </sst>
 </file>
@@ -697,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36EF922A-C188-1F43-B267-5D771EC01B6B}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -859,11 +862,17 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
+    <row r="14" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="6">
+        <v>45641</v>
+      </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="D14" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>

</xml_diff>

<commit_message>
Levencyclus taak volledig functioneel, van aanmaken tot het beoordelen. Veel styling wijzigingen en verbeteringen. Informatie pagina gemaakt waar volledige werking visueel is uitgelegd. Andere zaken en details staan in logboek.
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d5897c9615995d8/hogeschool/semester 7/ApplicatieArchete/ProjectAppArch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelte\Documents\KUL\AppArch\Project\ProjectAppArch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{75A0BCD9-CD6A-4DEE-B4C2-C7B58EDF3D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{360CC0A2-9AB0-41AD-821C-41C9230FF9B8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7442D339-8D3C-4AD3-9107-1EF751FDFDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15345" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Naam student 2:</t>
   </si>
@@ -275,6 +275,218 @@
   </si>
   <si>
     <t xml:space="preserve">klant kan user aan duiden op taak, taak waar een toewijzing op gebeurd kan niet meer geboden op worden en komen achteraan op de bord te staan. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">editTask.html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-&gt; hernoemd naar task.html (de naamgevings conventie is niet meer uniform, heb deze aangepast maar de rest zo gelaten) en css error gefixt en styling voorzien.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Index Pagina</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: naam owner weergegeven op klusje, bieden op klusje knop styling.  Zonder succes gezocht naar systeem om user names weer te geven op index pagina (join queries, meerdere queries combineren, etc). Count(offers) doet ook moeilijk, staat in comentaar in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>taskrepo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Toegewezen klusjes zijn ook van de homepagina afgehaald, hebben geen toegevoegde waarde van daar nog te staan. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Profile pagina</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Helemaal herstructureerd met nieuwe layout. Klusjesman en klant krijgen nu elk de juist taken op de juiste plaats te zien en kunnen hun vereiste acties uitvoeren op de taken (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/completeTask</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> en </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/finalizeTask</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">[maincontroller,taskcontroller] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>en</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> taskrepo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Volledig proces is functioneel van taak aanmaken tot het beoordelen, inclusief css styling, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To do</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Rating berekenen en ophalen voor Profile page klusjesman als pagina toekennen van task bij klant. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Info Pagina:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Informatie pagina gemaakt. Hier is de werking van de website uitgelegd voor zowel klant als klusjesman met visuele begeleiding. Project is bijna klaar!! (denk ik)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -700,19 +912,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36EF922A-C188-1F43-B267-5D771EC01B6B}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.25" customWidth="1"/>
-    <col min="2" max="2" width="23.875" customWidth="1"/>
-    <col min="3" max="3" width="27.125" customWidth="1"/>
+    <col min="1" max="1" width="36.19921875" customWidth="1"/>
+    <col min="2" max="2" width="23.8984375" customWidth="1"/>
+    <col min="3" max="3" width="27.09765625" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
@@ -720,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
@@ -728,7 +940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -742,7 +954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
@@ -754,7 +966,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -766,7 +978,7 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -778,7 +990,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="163.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="163.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -790,7 +1002,7 @@
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
@@ -802,7 +1014,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -814,7 +1026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -826,7 +1038,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="252" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="249.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
@@ -838,7 +1050,7 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
@@ -850,7 +1062,7 @@
       </c>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -862,7 +1074,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
@@ -874,245 +1086,251 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="8"/>
+    <row r="15" spans="1:4" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="6">
+        <v>45642</v>
+      </c>
+      <c r="C15" s="8">
+        <v>10.5</v>
+      </c>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="6"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="1"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="1"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="1"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="1"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="1"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="1"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="1"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="1"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D57" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
api op geboden, toeveogen van bod weg doen, algemene functie problemen op gelost
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelte\Documents\KUL\AppArch\Project\ProjectAppArch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d5897c9615995d8/hogeschool/semester 7/ApplicatieArchete/ProjectAppArch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7442D339-8D3C-4AD3-9107-1EF751FDFDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{7442D339-8D3C-4AD3-9107-1EF751FDFDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9D7758D-E48F-498B-B36A-B4AAF59DA561}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Naam student 2:</t>
   </si>
@@ -487,6 +489,12 @@
       </rPr>
       <t xml:space="preserve"> Informatie pagina gemaakt. Hier is de werking van de website uitgelegd voor zowel klant als klusjesman met visuele begeleiding. Project is bijna klaar!! (denk ik)</t>
     </r>
+  </si>
+  <si>
+    <t>na login pagina error weg gehaald, overlopen van alle funcionaliteiten en de functies die niet meer werken gefixt, rating laten weer geven en bod weg doen voor klusjes man</t>
+  </si>
+  <si>
+    <t>geboden functie via api</t>
   </si>
 </sst>
 </file>
@@ -913,18 +921,18 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.19921875" customWidth="1"/>
-    <col min="2" max="2" width="23.8984375" customWidth="1"/>
-    <col min="3" max="3" width="27.09765625" customWidth="1"/>
+    <col min="1" max="1" width="36.25" customWidth="1"/>
+    <col min="2" max="2" width="23.875" customWidth="1"/>
+    <col min="3" max="3" width="27.125" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
@@ -932,7 +940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
@@ -940,7 +948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -954,7 +962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
@@ -966,7 +974,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -978,7 +986,7 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -990,7 +998,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="163.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="163.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1002,7 +1010,7 @@
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
@@ -1014,7 +1022,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -1026,7 +1034,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -1038,7 +1046,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="249.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="252" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
@@ -1050,7 +1058,7 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
@@ -1062,7 +1070,7 @@
       </c>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1074,7 +1082,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
@@ -1086,7 +1094,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="408.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
@@ -1098,239 +1106,251 @@
       </c>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
+    <row r="16" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="6">
+        <v>45644</v>
+      </c>
       <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
+      <c r="D16" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="6">
+        <v>45645</v>
+      </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="6"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="1"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="1"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="1"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="1"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="1"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="1"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="1"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="1"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D57" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
error fix als klusjesman geen rating heeft. Rating als float opgehaald en verwerkt. Aantal bieders weergegeven op elke pagina en ook op info pagina aangepast. maincontroller profiel pagina aangepast zodat klusjesmannen juiste tasks zien. En nog veel meer, zie logboek :)
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d5897c9615995d8/hogeschool/semester 7/ApplicatieArchete/ProjectAppArch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelte\Documents\KUL\AppArch\Project\ProjectAppArch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{7442D339-8D3C-4AD3-9107-1EF751FDFDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9D7758D-E48F-498B-B36A-B4AAF59DA561}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890D5807-F4BF-4EB1-B2F8-82C2A148E5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Naam student 2:</t>
   </si>
@@ -495,6 +495,197 @@
   </si>
   <si>
     <t>geboden functie via api</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Profile Pagina &amp; geboden.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Als klusjesman nog geen ratings heeft, error bij ophalen van pagina -&gt; gefixt via try catch met (NA/5). Ook overal rating op 10 veranderd naar rating op 5 (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>geboden,info,review,...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[maincontroller]:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> code in maincontroller was aangepast voor ophalen van toegewezen klusjes via de OfferRepo, maar daardoor waren er bugs: Elke klusjesman die ooit geboden heeft op een task zag deze verschijnen op hun profiel in alle volgende fasen ookal hadden ze deze niet toegewezen gekregen. Zij konden deze ook markeren als uitgevoerd etc. Daarnaast waren er model variabelen aangepast op 1 plek maar niet op de andere waardoor de volledig afgewerkte klusjes niet meer verschenen -&gt; gefixt. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>geboden,review,..</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> website logo in de menubalk linksboven anders gelinkt in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>general.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zodat deze zichtbaar is op deze pagina's. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALLES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> code in commentaar weghalen in elke klasse/controller/... </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Index &amp; Profile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: GEBODEN task weergeeft aantal biedingen rechtsonder op postit. Enkel eigenaar kan info van klusjesmannen zien op toekenningspagina.  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALLES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nog is getest van start to finish + opgave nagelezen om te kijken of alles erin zit. Task deleten als er al geboden is nog toegevoegd. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RATING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Aangepast zodat het als float wordt berekend en weergegeven.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -588,7 +779,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -602,6 +793,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -920,19 +1114,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36EF922A-C188-1F43-B267-5D771EC01B6B}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.25" customWidth="1"/>
-    <col min="2" max="2" width="23.875" customWidth="1"/>
-    <col min="3" max="3" width="27.125" customWidth="1"/>
+    <col min="1" max="1" width="36.19921875" customWidth="1"/>
+    <col min="2" max="2" width="23.8984375" customWidth="1"/>
+    <col min="3" max="3" width="27.09765625" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
@@ -940,7 +1134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
@@ -948,7 +1142,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -962,7 +1156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
@@ -974,7 +1168,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -986,7 +1180,7 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -998,7 +1192,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="163.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="163.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1010,7 +1204,7 @@
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
@@ -1022,7 +1216,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -1034,7 +1228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -1046,7 +1240,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="252" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="249.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
@@ -1058,7 +1252,7 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
@@ -1070,7 +1264,7 @@
       </c>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1082,7 +1276,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
@@ -1094,7 +1288,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="408.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
@@ -1106,7 +1300,7 @@
       </c>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -1118,7 +1312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
@@ -1130,227 +1324,233 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="8"/>
+    <row r="18" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="6">
+        <v>45649</v>
+      </c>
+      <c r="C18" s="10">
+        <v>6</v>
+      </c>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="6"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="1"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="1"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="1"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="1"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="1"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="1"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="1"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="1"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D57" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
registratie systeem fix, role alleen nog maar authenticatie and verplaten van sommige urls
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelte\Documents\KUL\AppArch\Project\ProjectAppArch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d5897c9615995d8/hogeschool/semester 7/ApplicatieArchete/ProjectAppArch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890D5807-F4BF-4EB1-B2F8-82C2A148E5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{890D5807-F4BF-4EB1-B2F8-82C2A148E5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAE485D8-545F-486E-A3BB-32F0207C6D16}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15345" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Naam student 2:</t>
   </si>
@@ -686,6 +686,9 @@
       </rPr>
       <t>: Aangepast zodat het als float wordt berekend en weergegeven.</t>
     </r>
+  </si>
+  <si>
+    <t>registratie: als je niet alles invuld krijg je een error als het email adres al in database staat krijg je een error en het verplaten van urls met role ipv alles ingelogt alles door getest</t>
   </si>
 </sst>
 </file>
@@ -1115,18 +1118,18 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.19921875" customWidth="1"/>
-    <col min="2" max="2" width="23.8984375" customWidth="1"/>
-    <col min="3" max="3" width="27.09765625" customWidth="1"/>
+    <col min="1" max="1" width="36.25" customWidth="1"/>
+    <col min="2" max="2" width="23.875" customWidth="1"/>
+    <col min="3" max="3" width="27.125" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
@@ -1142,7 +1145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1156,7 +1159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
@@ -1168,7 +1171,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1180,7 +1183,7 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -1192,7 +1195,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="163.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="163.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1204,7 +1207,7 @@
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
@@ -1216,7 +1219,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -1240,7 +1243,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="249.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="252" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
@@ -1252,7 +1255,7 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
@@ -1264,7 +1267,7 @@
       </c>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1276,7 +1279,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
@@ -1288,7 +1291,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="408.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
@@ -1300,7 +1303,7 @@
       </c>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4" ht="78" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -1312,7 +1315,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
@@ -1324,7 +1327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>21</v>
       </c>
@@ -1336,221 +1339,227 @@
       </c>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
+    <row r="19" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="6">
+        <v>45655</v>
+      </c>
       <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D19" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="6"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="1"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="1"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="1"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="1"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="1"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="1"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="1"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="1"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D57" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PROJECT IS AF! Rating afgerond tot 1 cijfer na de komma. Kleine quality of life aanpassing aan info pagina (klusje nuttige naam gegeven) en registratie error iets korter gemaakt. Alles nog eens overlopen van begin tot einde (+opgave), alles zit er in!
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d5897c9615995d8/hogeschool/semester 7/ApplicatieArchete/ProjectAppArch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelte\Documents\KUL\AppArch\Project\ProjectAppArch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{890D5807-F4BF-4EB1-B2F8-82C2A148E5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAE485D8-545F-486E-A3BB-32F0207C6D16}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EB0352-15A0-491F-BDBE-F4DFA804C2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="28800" windowHeight="15345" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Naam student 2:</t>
   </si>
@@ -689,6 +689,31 @@
   </si>
   <si>
     <t>registratie: als je niet alles invuld krijg je een error als het email adres al in database staat krijg je een error en het verplaten van urls met role ipv alles ingelogt alles door getest</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PROJECT IS AF!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Rating afgerond tot 1 cijfer na de komma. Kleine quality of life aanpassing aan info pagina (klusje nuttige naam gegeven) en registratie error iets korter gemaakt. Alles nog eens overlopen van begin tot einde (+opgave), alles zit er in!</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -698,7 +723,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -724,6 +749,16 @@
     </font>
     <font>
       <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1121,15 +1156,15 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.25" customWidth="1"/>
-    <col min="2" max="2" width="23.875" customWidth="1"/>
-    <col min="3" max="3" width="27.125" customWidth="1"/>
+    <col min="1" max="1" width="36.19921875" customWidth="1"/>
+    <col min="2" max="2" width="23.8984375" customWidth="1"/>
+    <col min="3" max="3" width="27.09765625" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1137,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
@@ -1145,7 +1180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1159,7 +1194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
@@ -1171,7 +1206,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1183,7 +1218,7 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -1195,7 +1230,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="163.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="163.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1207,7 +1242,7 @@
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
@@ -1219,7 +1254,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -1231,7 +1266,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -1243,7 +1278,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="252" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="249.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
@@ -1255,7 +1290,7 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
@@ -1267,7 +1302,7 @@
       </c>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1279,7 +1314,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
@@ -1291,7 +1326,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="408.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
@@ -1303,7 +1338,7 @@
       </c>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -1315,7 +1350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
@@ -1327,7 +1362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>21</v>
       </c>
@@ -1339,7 +1374,7 @@
       </c>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="78" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1351,215 +1386,221 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="8"/>
+    <row r="20" spans="1:4" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="6">
+        <v>45656</v>
+      </c>
+      <c r="C20" s="8">
+        <v>0.5</v>
+      </c>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="6"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="1"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="1"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="1"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="1"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="1"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="1"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="1"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="1"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D57" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
warnings weg gedaan en comentaar code weg en database foto update
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelte\Documents\KUL\AppArch\Project\ProjectAppArch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d5897c9615995d8/hogeschool/semester 7/ApplicatieArchete/ProjectAppArch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EB0352-15A0-491F-BDBE-F4DFA804C2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{F3EB0352-15A0-491F-BDBE-F4DFA804C2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{483F0275-8D5A-4CEA-93C0-373C6514AE3C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1152,19 +1152,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36EF922A-C188-1F43-B267-5D771EC01B6B}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.19921875" customWidth="1"/>
-    <col min="2" max="2" width="23.8984375" customWidth="1"/>
-    <col min="3" max="3" width="27.09765625" customWidth="1"/>
+    <col min="1" max="1" width="36.25" customWidth="1"/>
+    <col min="2" max="2" width="23.875" customWidth="1"/>
+    <col min="3" max="3" width="27.125" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1218,7 +1218,7 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="163.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="163.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1242,7 +1242,7 @@
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="249.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="252" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="408.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
@@ -1338,7 +1338,7 @@
       </c>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4" ht="78" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>21</v>
       </c>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" ht="78" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1398,209 +1398,209 @@
       </c>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="6"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="1"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="1"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="1"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="1"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="1"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="1"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="1"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="1"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D57" s="3"/>
     </row>
   </sheetData>

</xml_diff>